<commit_message>
updated scripts to create complete SISEPUEDE class
</commit_message>
<xml_diff>
--- a/ref/ingestion/demo/model_input_variables_en_demo.xlsx
+++ b/ref/ingestion/demo/model_input_variables_en_demo.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39D88A7-4685-2A44-AFFC-55850EF0A194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C18F71F-9581-4F43-9BF6-A8CD4A6F098B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="480" windowWidth="23460" windowHeight="20620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7680" yWindow="460" windowWidth="23460" windowHeight="20620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
-    <sheet name="strategy_id-1" sheetId="2" r:id="rId2"/>
+    <sheet name="strategy_id-2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'strategy_id-0'!$A$1:$AS$811</definedName>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="907">
   <si>
     <t>subsector</t>
   </si>
@@ -3186,8 +3186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS851"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="107" workbookViewId="0">
-      <selection activeCell="G111" sqref="G111"/>
+    <sheetView topLeftCell="A257" zoomScale="107" workbookViewId="0">
+      <selection activeCell="A271" sqref="A271:XFD282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -107103,11 +107103,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AU1"/>
+  <dimension ref="A1:AU6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AQ4" sqref="AQ4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -107250,6 +107255,646 @@
       </c>
       <c r="AU1" s="1" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>653</v>
+      </c>
+      <c r="B2" t="s">
+        <v>791</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>-999</v>
+      </c>
+      <c r="K2">
+        <v>-999</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0.5</v>
+      </c>
+      <c r="Y2">
+        <v>0.5</v>
+      </c>
+      <c r="Z2">
+        <v>0.5</v>
+      </c>
+      <c r="AA2">
+        <v>0.5</v>
+      </c>
+      <c r="AB2">
+        <v>0.5</v>
+      </c>
+      <c r="AC2">
+        <v>0.5</v>
+      </c>
+      <c r="AD2">
+        <v>0.5</v>
+      </c>
+      <c r="AE2">
+        <v>0.5</v>
+      </c>
+      <c r="AF2">
+        <v>0.5</v>
+      </c>
+      <c r="AG2">
+        <v>0.5</v>
+      </c>
+      <c r="AH2">
+        <v>0.5</v>
+      </c>
+      <c r="AI2">
+        <v>0.5</v>
+      </c>
+      <c r="AJ2">
+        <v>0.5</v>
+      </c>
+      <c r="AK2">
+        <v>0.5</v>
+      </c>
+      <c r="AL2">
+        <v>0.5</v>
+      </c>
+      <c r="AM2">
+        <v>0.5</v>
+      </c>
+      <c r="AN2">
+        <v>0.5</v>
+      </c>
+      <c r="AO2">
+        <v>0.5</v>
+      </c>
+      <c r="AP2">
+        <v>0.5</v>
+      </c>
+      <c r="AQ2">
+        <v>0.5</v>
+      </c>
+      <c r="AR2">
+        <v>0.5</v>
+      </c>
+      <c r="AS2">
+        <v>0.5</v>
+      </c>
+      <c r="AT2">
+        <v>0.5</v>
+      </c>
+      <c r="AU2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>653</v>
+      </c>
+      <c r="B3" t="s">
+        <v>792</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>-999</v>
+      </c>
+      <c r="K3">
+        <v>-999</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0.1</v>
+      </c>
+      <c r="Y3">
+        <v>0.1</v>
+      </c>
+      <c r="Z3">
+        <v>0.1</v>
+      </c>
+      <c r="AA3">
+        <v>0.1</v>
+      </c>
+      <c r="AB3">
+        <v>0.1</v>
+      </c>
+      <c r="AC3">
+        <v>0.1</v>
+      </c>
+      <c r="AD3">
+        <v>0.1</v>
+      </c>
+      <c r="AE3">
+        <v>0.1</v>
+      </c>
+      <c r="AF3">
+        <v>0.1</v>
+      </c>
+      <c r="AG3">
+        <v>0.1</v>
+      </c>
+      <c r="AH3">
+        <v>0.1</v>
+      </c>
+      <c r="AI3">
+        <v>0.1</v>
+      </c>
+      <c r="AJ3">
+        <v>0.1</v>
+      </c>
+      <c r="AK3">
+        <v>0.1</v>
+      </c>
+      <c r="AL3">
+        <v>0.1</v>
+      </c>
+      <c r="AM3">
+        <v>0.1</v>
+      </c>
+      <c r="AN3">
+        <v>0.1</v>
+      </c>
+      <c r="AO3">
+        <v>0.1</v>
+      </c>
+      <c r="AP3">
+        <v>0.1</v>
+      </c>
+      <c r="AQ3">
+        <v>0.1</v>
+      </c>
+      <c r="AR3">
+        <v>0.1</v>
+      </c>
+      <c r="AS3">
+        <v>0.1</v>
+      </c>
+      <c r="AT3">
+        <v>0.1</v>
+      </c>
+      <c r="AU3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>653</v>
+      </c>
+      <c r="B4" t="s">
+        <v>794</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>-999</v>
+      </c>
+      <c r="K4">
+        <v>-999</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0.1</v>
+      </c>
+      <c r="Y4">
+        <v>0.1</v>
+      </c>
+      <c r="Z4">
+        <v>0.1</v>
+      </c>
+      <c r="AA4">
+        <v>0.1</v>
+      </c>
+      <c r="AB4">
+        <v>0.1</v>
+      </c>
+      <c r="AC4">
+        <v>0.1</v>
+      </c>
+      <c r="AD4">
+        <v>0.1</v>
+      </c>
+      <c r="AE4">
+        <v>0.1</v>
+      </c>
+      <c r="AF4">
+        <v>0.1</v>
+      </c>
+      <c r="AG4">
+        <v>0.1</v>
+      </c>
+      <c r="AH4">
+        <v>0.1</v>
+      </c>
+      <c r="AI4">
+        <v>0.1</v>
+      </c>
+      <c r="AJ4">
+        <v>0.1</v>
+      </c>
+      <c r="AK4">
+        <v>0.1</v>
+      </c>
+      <c r="AL4">
+        <v>0.1</v>
+      </c>
+      <c r="AM4">
+        <v>0.1</v>
+      </c>
+      <c r="AN4">
+        <v>0.1</v>
+      </c>
+      <c r="AO4">
+        <v>0.1</v>
+      </c>
+      <c r="AP4">
+        <v>0.1</v>
+      </c>
+      <c r="AQ4">
+        <v>0.1</v>
+      </c>
+      <c r="AR4">
+        <v>0.1</v>
+      </c>
+      <c r="AS4">
+        <v>0.1</v>
+      </c>
+      <c r="AT4">
+        <v>0.1</v>
+      </c>
+      <c r="AU4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>653</v>
+      </c>
+      <c r="B5" t="s">
+        <v>796</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>-999</v>
+      </c>
+      <c r="K5">
+        <v>-999</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0.5</v>
+      </c>
+      <c r="Y5">
+        <v>0.5</v>
+      </c>
+      <c r="Z5">
+        <v>0.5</v>
+      </c>
+      <c r="AA5">
+        <v>0.5</v>
+      </c>
+      <c r="AB5">
+        <v>0.5</v>
+      </c>
+      <c r="AC5">
+        <v>0.5</v>
+      </c>
+      <c r="AD5">
+        <v>0.5</v>
+      </c>
+      <c r="AE5">
+        <v>0.5</v>
+      </c>
+      <c r="AF5">
+        <v>0.5</v>
+      </c>
+      <c r="AG5">
+        <v>0.5</v>
+      </c>
+      <c r="AH5">
+        <v>0.5</v>
+      </c>
+      <c r="AI5">
+        <v>0.5</v>
+      </c>
+      <c r="AJ5">
+        <v>0.5</v>
+      </c>
+      <c r="AK5">
+        <v>0.5</v>
+      </c>
+      <c r="AL5">
+        <v>0.5</v>
+      </c>
+      <c r="AM5">
+        <v>0.5</v>
+      </c>
+      <c r="AN5">
+        <v>0.5</v>
+      </c>
+      <c r="AO5">
+        <v>0.5</v>
+      </c>
+      <c r="AP5">
+        <v>0.5</v>
+      </c>
+      <c r="AQ5">
+        <v>0.5</v>
+      </c>
+      <c r="AR5">
+        <v>0.5</v>
+      </c>
+      <c r="AS5">
+        <v>0.5</v>
+      </c>
+      <c r="AT5">
+        <v>0.5</v>
+      </c>
+      <c r="AU5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>653</v>
+      </c>
+      <c r="B6" t="s">
+        <v>798</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>-999</v>
+      </c>
+      <c r="K6">
+        <v>-999</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0.5</v>
+      </c>
+      <c r="Y6">
+        <v>0.5</v>
+      </c>
+      <c r="Z6">
+        <v>0.5</v>
+      </c>
+      <c r="AA6">
+        <v>0.5</v>
+      </c>
+      <c r="AB6">
+        <v>0.5</v>
+      </c>
+      <c r="AC6">
+        <v>0.5</v>
+      </c>
+      <c r="AD6">
+        <v>0.5</v>
+      </c>
+      <c r="AE6">
+        <v>0.5</v>
+      </c>
+      <c r="AF6">
+        <v>0.5</v>
+      </c>
+      <c r="AG6">
+        <v>0.5</v>
+      </c>
+      <c r="AH6">
+        <v>0.5</v>
+      </c>
+      <c r="AI6">
+        <v>0.5</v>
+      </c>
+      <c r="AJ6">
+        <v>0.5</v>
+      </c>
+      <c r="AK6">
+        <v>0.5</v>
+      </c>
+      <c r="AL6">
+        <v>0.5</v>
+      </c>
+      <c r="AM6">
+        <v>0.5</v>
+      </c>
+      <c r="AN6">
+        <v>0.5</v>
+      </c>
+      <c r="AO6">
+        <v>0.5</v>
+      </c>
+      <c r="AP6">
+        <v>0.5</v>
+      </c>
+      <c r="AQ6">
+        <v>0.5</v>
+      </c>
+      <c r="AR6">
+        <v>0.5</v>
+      </c>
+      <c r="AS6">
+        <v>0.5</v>
+      </c>
+      <c r="AT6">
+        <v>0.5</v>
+      </c>
+      <c r="AU6">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug in energy model and added/cleaned output variables
</commit_message>
<xml_diff>
--- a/ref/ingestion/demo/model_input_variables_en_demo.xlsx
+++ b/ref/ingestion/demo/model_input_variables_en_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C18F71F-9581-4F43-9BF6-A8CD4A6F098B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD3FB5D-2BCF-384C-9A71-7FB76596B9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="460" windowWidth="23460" windowHeight="20620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7680" yWindow="460" windowWidth="23460" windowHeight="20620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -3186,8 +3186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS851"/>
   <sheetViews>
-    <sheetView topLeftCell="A257" zoomScale="107" workbookViewId="0">
-      <selection activeCell="A271" sqref="A271:XFD282"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -107105,7 +107105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AU6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="AQ4" sqref="AQ4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated renewable efficiency factors in fake data
</commit_message>
<xml_diff>
--- a/ref/ingestion/demo/model_input_variables_en_demo.xlsx
+++ b/ref/ingestion/demo/model_input_variables_en_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BA24FA-DD78-D94E-842A-9D5BD5B06778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443DF02B-C706-E742-9583-CF48F86BCCF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-840" yWindow="520" windowWidth="17300" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34440" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -3252,8 +3252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS873"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="111" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="111" workbookViewId="0">
+      <selection activeCell="L147" sqref="L147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21402,112 +21402,112 @@
         <v>1.2</v>
       </c>
       <c r="J149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="K149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="L149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="M149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="N149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="O149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="P149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="Q149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="R149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="S149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="T149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="U149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="V149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="W149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="X149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="Y149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="Z149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AA149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AB149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AC149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AD149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AE149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AF149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AG149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AH149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AI149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AJ149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AK149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AL149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AM149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AN149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AO149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AP149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AQ149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AR149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="AS149">
-        <v>0.35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:45" x14ac:dyDescent="0.2">
@@ -21524,112 +21524,112 @@
         <v>1.2</v>
       </c>
       <c r="J150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="K150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="L150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="M150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="N150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="O150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="P150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="Q150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="R150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="S150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="T150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="U150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="V150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="W150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="X150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="Y150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="Z150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AA150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AB150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AC150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AD150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AE150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AF150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AG150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AH150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AI150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AJ150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AK150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AL150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AM150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AN150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AO150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AP150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AQ150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AR150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="AS150">
-        <v>0.85</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:45" x14ac:dyDescent="0.2">
@@ -21768,112 +21768,112 @@
         <v>1.2</v>
       </c>
       <c r="J152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="K152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="L152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="M152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="N152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="O152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="P152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="Q152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="R152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="S152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="T152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="U152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="V152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="W152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="X152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="Y152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="Z152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AA152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AB152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AC152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AD152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AE152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AF152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AG152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AH152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AI152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AJ152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AK152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AL152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AM152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AN152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AO152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AP152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AQ152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AR152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AS152">
-        <v>0.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:45" x14ac:dyDescent="0.2">
@@ -22012,112 +22012,112 @@
         <v>1.2</v>
       </c>
       <c r="J154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="K154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="L154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="M154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="N154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="O154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="P154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="Q154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="R154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="S154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="T154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="U154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="V154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="W154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="X154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="Y154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="Z154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AA154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AB154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AC154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AD154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AE154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AF154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AG154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AH154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AI154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AJ154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AK154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AL154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AM154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AN154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AO154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AP154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AQ154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AR154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="AS154">
-        <v>0.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:45" x14ac:dyDescent="0.2">
@@ -22256,112 +22256,112 @@
         <v>1.2</v>
       </c>
       <c r="J156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="K156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="L156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="M156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="N156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="O156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="P156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="Q156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="R156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="S156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="T156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="U156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="V156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="W156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="X156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="Y156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="Z156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AA156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AB156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AC156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AD156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AE156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AF156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AG156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AH156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AI156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AJ156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AK156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AL156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AM156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AN156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AO156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AP156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AQ156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AR156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="AS156">
-        <v>0.375</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:45" x14ac:dyDescent="0.2">

</xml_diff>